<commit_message>
Graphic adjustments for report
</commit_message>
<xml_diff>
--- a/Data_dictionary.xlsx
+++ b/Data_dictionary.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juand\Documentos\UTS - Data Science and Innovation\Spring Session 2024\Statistical Thinking for Data Science\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentutsedu-my.sharepoint.com/personal/juan_d_balseroleon_student_uts_edu_au/Documents/UTS - Data Science and Innovation/Spring Session 2024/Statistical Thinking for Data Science/Assignment 3/STDS_at3/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7138EE-555A-484B-9372-1598CD852D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -504,7 +504,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>